<commit_message>
font warning in schematic
</commit_message>
<xml_diff>
--- a/-PCB-/SUMEC_MK_IV/bom/MK_IV bom.xlsx
+++ b/-PCB-/SUMEC_MK_IV/bom/MK_IV bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\Sumec-MiniSumo\-PCB-\SUMEC_MK_IV\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86311BEF-AC7C-4538-9DB4-16928A6D7370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24F4747-D9B1-414D-BB60-4EEA114D8C98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="123">
   <si>
     <t>Id</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>Red LED, 20mA 1.9V, 0805</t>
+  </si>
+  <si>
+    <t>45.3k, 125mW, vishay</t>
+  </si>
+  <si>
+    <t>Datasheet says it 0.6-7V output, desc.6-7V</t>
   </si>
 </sst>
 </file>
@@ -579,7 +585,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="42">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -804,12 +810,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1032,11 +1032,11 @@
     <xf numFmtId="0" fontId="20" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1417,7 +1417,7 @@
   <dimension ref="A1:J78"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="73" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1498,7 +1498,9 @@
       <c r="E3" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="F3" s="15"/>
+      <c r="F3" s="16" t="s">
+        <v>121</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
@@ -2026,7 +2028,9 @@
       <c r="F27" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="G27" s="14"/>
+      <c r="G27" s="14" t="s">
+        <v>122</v>
+      </c>
       <c r="H27" s="11"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -2163,7 +2167,7 @@
       <c r="E35" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F35" s="16" t="s">
+      <c r="F35" s="15" t="s">
         <v>120</v>
       </c>
       <c r="G35" s="1"/>
@@ -2365,8 +2369,9 @@
     <hyperlink ref="F35" r:id="rId24" display="Red LED, 20mA 1.9V, 0805, mouser" xr:uid="{631A8368-CC6E-497A-BA50-9C7465C90281}"/>
     <hyperlink ref="F36" r:id="rId25" display="Yellow LED, 20mA, 1.9V, 0805, mouser" xr:uid="{50E4AE87-8DC6-4D9C-8956-48E26D8347E9}"/>
     <hyperlink ref="F37" r:id="rId26" display="Green-Yellow LED, 20mA, 1.9V, mouser" xr:uid="{EB8941BD-8C79-4349-A76B-A0A9B67E34C1}"/>
+    <hyperlink ref="F3" r:id="rId27" xr:uid="{D4D1F7D7-BE9E-4734-96F3-48B07F1A3520}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId28"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Jonas + Savva motor test code
</commit_message>
<xml_diff>
--- a/-PCB-/SUMEC_MK_IV/bom/MK_IV bom.xlsx
+++ b/-PCB-/SUMEC_MK_IV/bom/MK_IV bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MenMe\GitHub\Sumec-MiniSumo\-PCB-\SUMEC_MK_IV\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD5E012-F036-42F0-8B4C-4660927EDD91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23F64905-20AC-47B3-9376-298AC0807CCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1488,8 +1488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B36" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F51" sqref="F46:F51"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="64" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>